<commit_message>
Q3 2021 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/236e6b124acc9753/Documents/Indicators/Data/Fiscal Data/NG Outstanding Debt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{B75CE391-019B-4544-8B21-71DBF0746443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EF593C5-F8CE-4B77-8C2E-820CC7A7A5DC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F94AF54-5CBC-4BA7-A1EC-9EB2C23072E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="1620" windowWidth="13830" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12855" yWindow="1365" windowWidth="15540" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="14" r:id="rId1"/>
@@ -1137,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9061F1E7-8550-4A80-8C52-E95CE64AC367}">
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43:M44"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1307,15 +1307,15 @@
       </c>
       <c r="N8" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12054772</v>
       </c>
       <c r="O8" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12074737</v>
       </c>
       <c r="P8" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12349910</v>
       </c>
       <c r="Q8" s="17">
         <f t="shared" si="0"/>
@@ -1387,15 +1387,15 @@
       </c>
       <c r="N10" s="101">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11610465</v>
       </c>
       <c r="O10" s="101">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11642519</v>
       </c>
       <c r="P10" s="101">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11917047</v>
       </c>
       <c r="Q10" s="101">
         <f t="shared" si="1"/>
@@ -1467,15 +1467,15 @@
       </c>
       <c r="N12" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8119598</v>
       </c>
       <c r="O12" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8220304</v>
       </c>
       <c r="P12" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8387753</v>
       </c>
       <c r="Q12" s="23">
         <f t="shared" si="2"/>
@@ -1526,15 +1526,15 @@
       </c>
       <c r="N13" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="O13" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="P13" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="Q13" s="23">
         <f t="shared" si="3"/>
@@ -1585,15 +1585,15 @@
       </c>
       <c r="N14" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="O14" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="P14" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="Q14" s="25">
         <f t="shared" si="4"/>
@@ -1636,9 +1636,15 @@
       <c r="M15" s="26">
         <v>540156</v>
       </c>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
+      <c r="N15" s="26">
+        <v>540156</v>
+      </c>
+      <c r="O15" s="26">
+        <v>540156</v>
+      </c>
+      <c r="P15" s="26">
+        <v>540156</v>
+      </c>
       <c r="Q15" s="26"/>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -1671,9 +1677,15 @@
       <c r="M16" s="26">
         <v>156</v>
       </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
+      <c r="N16" s="26">
+        <v>156</v>
+      </c>
+      <c r="O16" s="26">
+        <v>156</v>
+      </c>
+      <c r="P16" s="26">
+        <v>156</v>
+      </c>
       <c r="Q16" s="26"/>
       <c r="R16" s="26"/>
       <c r="S16" s="26"/>
@@ -1706,9 +1718,15 @@
       <c r="M17" s="26">
         <v>540000</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="N17" s="26">
+        <v>540000</v>
+      </c>
+      <c r="O17" s="26">
+        <v>540000</v>
+      </c>
+      <c r="P17" s="26">
+        <v>540000</v>
+      </c>
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26"/>
@@ -1741,9 +1759,15 @@
       <c r="M18" s="26">
         <v>0</v>
       </c>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
+      <c r="N18" s="26">
+        <v>0</v>
+      </c>
+      <c r="O18" s="26">
+        <v>0</v>
+      </c>
+      <c r="P18" s="26">
+        <v>0</v>
+      </c>
       <c r="Q18" s="26"/>
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
@@ -1835,9 +1859,15 @@
       <c r="M20" s="26">
         <v>0</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
+      <c r="N20" s="26">
+        <v>0</v>
+      </c>
+      <c r="O20" s="26">
+        <v>0</v>
+      </c>
+      <c r="P20" s="26">
+        <v>0</v>
+      </c>
       <c r="Q20" s="26"/>
       <c r="R20" s="26"/>
       <c r="S20" s="26"/>
@@ -1870,9 +1900,15 @@
       <c r="M21" s="26">
         <v>0</v>
       </c>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
+      <c r="N21" s="26">
+        <v>0</v>
+      </c>
+      <c r="O21" s="26">
+        <v>0</v>
+      </c>
+      <c r="P21" s="26">
+        <v>0</v>
+      </c>
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
@@ -1992,9 +2028,15 @@
       <c r="M25" s="28">
         <v>7398401</v>
       </c>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
+      <c r="N25" s="28">
+        <v>7579442</v>
+      </c>
+      <c r="O25" s="28">
+        <v>7680148</v>
+      </c>
+      <c r="P25" s="28">
+        <v>7847597</v>
+      </c>
       <c r="Q25" s="28"/>
       <c r="R25" s="28"/>
       <c r="S25" s="28"/>
@@ -2056,15 +2098,15 @@
       </c>
       <c r="N27" s="23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3490867</v>
       </c>
       <c r="O27" s="23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3422215</v>
       </c>
       <c r="P27" s="23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3529294</v>
       </c>
       <c r="Q27" s="23">
         <f t="shared" si="6"/>
@@ -2115,15 +2157,15 @@
       </c>
       <c r="N28" s="25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1471994</v>
       </c>
       <c r="O28" s="25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1471188</v>
       </c>
       <c r="P28" s="25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1542150</v>
       </c>
       <c r="Q28" s="25">
         <f t="shared" si="7"/>
@@ -2174,15 +2216,15 @@
       </c>
       <c r="N29" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1471994</v>
       </c>
       <c r="O29" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1471188</v>
       </c>
       <c r="P29" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1542150</v>
       </c>
       <c r="Q29" s="30">
         <f t="shared" si="8"/>
@@ -2225,9 +2267,15 @@
       <c r="M30" s="28">
         <v>1398146</v>
       </c>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="28"/>
+      <c r="N30" s="28">
+        <v>1454336</v>
+      </c>
+      <c r="O30" s="28">
+        <v>1453960</v>
+      </c>
+      <c r="P30" s="28">
+        <v>1525143</v>
+      </c>
       <c r="Q30" s="28"/>
       <c r="R30" s="28"/>
       <c r="S30" s="28"/>
@@ -2260,9 +2308,15 @@
       <c r="M31" s="28">
         <v>16918</v>
       </c>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="28"/>
+      <c r="N31" s="28">
+        <v>17658</v>
+      </c>
+      <c r="O31" s="28">
+        <v>17228</v>
+      </c>
+      <c r="P31" s="28">
+        <v>17007</v>
+      </c>
       <c r="Q31" s="28"/>
       <c r="R31" s="28"/>
       <c r="S31" s="28"/>
@@ -2351,9 +2405,15 @@
       <c r="M34" s="28">
         <v>1812412</v>
       </c>
-      <c r="N34" s="28"/>
-      <c r="O34" s="28"/>
-      <c r="P34" s="28"/>
+      <c r="N34" s="28">
+        <v>2018873</v>
+      </c>
+      <c r="O34" s="28">
+        <v>1951027</v>
+      </c>
+      <c r="P34" s="28">
+        <v>1987144</v>
+      </c>
       <c r="Q34" s="28"/>
       <c r="R34" s="28"/>
       <c r="S34" s="28"/>
@@ -2432,15 +2492,15 @@
       </c>
       <c r="N37" s="105">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>444307</v>
       </c>
       <c r="O37" s="105">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>432218</v>
       </c>
       <c r="P37" s="105">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>432863</v>
       </c>
       <c r="Q37" s="105">
         <f t="shared" si="9"/>
@@ -2491,15 +2551,15 @@
       </c>
       <c r="N38" s="35">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>242653</v>
       </c>
       <c r="O38" s="35">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>233113</v>
       </c>
       <c r="P38" s="35">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>232969</v>
       </c>
       <c r="Q38" s="35">
         <f t="shared" si="10"/>
@@ -2542,9 +2602,15 @@
       <c r="M39" s="38">
         <v>243940</v>
       </c>
-      <c r="N39" s="38"/>
-      <c r="O39" s="38"/>
-      <c r="P39" s="38"/>
+      <c r="N39" s="38">
+        <v>242517</v>
+      </c>
+      <c r="O39" s="38">
+        <v>232977</v>
+      </c>
+      <c r="P39" s="38">
+        <v>232833</v>
+      </c>
       <c r="Q39" s="38"/>
       <c r="R39" s="38"/>
       <c r="S39" s="38"/>
@@ -2577,9 +2643,15 @@
       <c r="M40" s="38">
         <v>136</v>
       </c>
-      <c r="N40" s="38"/>
-      <c r="O40" s="38"/>
-      <c r="P40" s="38"/>
+      <c r="N40" s="38">
+        <v>136</v>
+      </c>
+      <c r="O40" s="38">
+        <v>136</v>
+      </c>
+      <c r="P40" s="38">
+        <v>136</v>
+      </c>
       <c r="Q40" s="38"/>
       <c r="R40" s="38"/>
       <c r="S40" s="38"/>
@@ -2640,15 +2712,15 @@
       </c>
       <c r="N42" s="35">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>201654</v>
       </c>
       <c r="O42" s="35">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>199105</v>
       </c>
       <c r="P42" s="35">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>199894</v>
       </c>
       <c r="Q42" s="35">
         <f t="shared" si="11"/>
@@ -2685,9 +2757,15 @@
       <c r="M43" s="38">
         <v>190357</v>
       </c>
-      <c r="N43" s="38"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="38"/>
+      <c r="N43" s="38">
+        <v>197357</v>
+      </c>
+      <c r="O43" s="38">
+        <v>194848</v>
+      </c>
+      <c r="P43" s="38">
+        <v>195542</v>
+      </c>
       <c r="Q43" s="38"/>
       <c r="R43" s="38"/>
       <c r="S43" s="38"/>
@@ -2714,9 +2792,15 @@
       <c r="M44" s="38">
         <v>4167</v>
       </c>
-      <c r="N44" s="38"/>
-      <c r="O44" s="38"/>
-      <c r="P44" s="38"/>
+      <c r="N44" s="38">
+        <v>4297</v>
+      </c>
+      <c r="O44" s="38">
+        <v>4257</v>
+      </c>
+      <c r="P44" s="38">
+        <v>4352</v>
+      </c>
       <c r="Q44" s="38"/>
       <c r="R44" s="38"/>
       <c r="S44" s="38"/>

</xml_diff>

<commit_message>
Q4 2021 Fiscal Data udpate
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F94AF54-5CBC-4BA7-A1EC-9EB2C23072E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C6E019-41C5-4DB7-91D5-388104184A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12855" yWindow="1365" windowWidth="15540" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="14" r:id="rId1"/>
@@ -1319,15 +1319,15 @@
       </c>
       <c r="Q8" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12397996</v>
       </c>
       <c r="R8" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12349675</v>
       </c>
       <c r="S8" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12152466</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="18" customFormat="1">
@@ -1399,15 +1399,15 @@
       </c>
       <c r="Q10" s="101">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11971532</v>
       </c>
       <c r="R10" s="101">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11931828</v>
       </c>
       <c r="S10" s="101">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11728549</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="6.95" customHeight="1">
@@ -1479,15 +1479,15 @@
       </c>
       <c r="Q12" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8468408</v>
       </c>
       <c r="R12" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8441502</v>
       </c>
       <c r="S12" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8170414</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1538,15 +1538,15 @@
       </c>
       <c r="Q13" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="R13" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="S13" s="23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1597,15 +1597,15 @@
       </c>
       <c r="Q14" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="R14" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>540156</v>
       </c>
       <c r="S14" s="25">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1645,9 +1645,15 @@
       <c r="P15" s="26">
         <v>540156</v>
       </c>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
+      <c r="Q15" s="26">
+        <v>540156</v>
+      </c>
+      <c r="R15" s="26">
+        <v>540156</v>
+      </c>
+      <c r="S15" s="26">
+        <v>156</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="14"/>
@@ -1686,9 +1692,15 @@
       <c r="P16" s="26">
         <v>156</v>
       </c>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
+      <c r="Q16" s="26">
+        <v>156</v>
+      </c>
+      <c r="R16" s="26">
+        <v>156</v>
+      </c>
+      <c r="S16" s="26">
+        <v>156</v>
+      </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="14"/>
@@ -1727,9 +1739,15 @@
       <c r="P17" s="26">
         <v>540000</v>
       </c>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
+      <c r="Q17" s="26">
+        <v>540000</v>
+      </c>
+      <c r="R17" s="26">
+        <v>540000</v>
+      </c>
+      <c r="S17" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="14"/>
@@ -1768,9 +1786,15 @@
       <c r="P18" s="26">
         <v>0</v>
       </c>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
+      <c r="Q18" s="26">
+        <v>0</v>
+      </c>
+      <c r="R18" s="26">
+        <v>0</v>
+      </c>
+      <c r="S18" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="14"/>
@@ -1868,9 +1892,15 @@
       <c r="P20" s="26">
         <v>0</v>
       </c>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
+      <c r="Q20" s="26">
+        <v>0</v>
+      </c>
+      <c r="R20" s="26">
+        <v>0</v>
+      </c>
+      <c r="S20" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="14"/>
@@ -1909,9 +1939,15 @@
       <c r="P21" s="26">
         <v>0</v>
       </c>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
+      <c r="Q21" s="26">
+        <v>0</v>
+      </c>
+      <c r="R21" s="26">
+        <v>0</v>
+      </c>
+      <c r="S21" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:19" hidden="1">
       <c r="A22" s="14"/>
@@ -2037,9 +2073,15 @@
       <c r="P25" s="28">
         <v>7847597</v>
       </c>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
+      <c r="Q25" s="28">
+        <v>7928252</v>
+      </c>
+      <c r="R25" s="28">
+        <v>7901346</v>
+      </c>
+      <c r="S25" s="28">
+        <v>8170258</v>
+      </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="14"/>
@@ -2110,15 +2152,15 @@
       </c>
       <c r="Q27" s="23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3503124</v>
       </c>
       <c r="R27" s="23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3490326</v>
       </c>
       <c r="S27" s="23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3558135</v>
       </c>
     </row>
     <row r="28" spans="1:19" s="29" customFormat="1">
@@ -2169,15 +2211,15 @@
       </c>
       <c r="Q28" s="25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1529576</v>
       </c>
       <c r="R28" s="25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1527793</v>
       </c>
       <c r="S28" s="25">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1574246</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -2228,15 +2270,15 @@
       </c>
       <c r="Q29" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1529576</v>
       </c>
       <c r="R29" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1527793</v>
       </c>
       <c r="S29" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1574246</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -2276,9 +2318,15 @@
       <c r="P30" s="28">
         <v>1525143</v>
       </c>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="28"/>
-      <c r="S30" s="28"/>
+      <c r="Q30" s="28">
+        <v>1513279</v>
+      </c>
+      <c r="R30" s="28">
+        <v>1511439</v>
+      </c>
+      <c r="S30" s="28">
+        <v>1558131</v>
+      </c>
     </row>
     <row r="31" spans="1:19">
       <c r="A31" s="14"/>
@@ -2317,9 +2365,15 @@
       <c r="P31" s="28">
         <v>17007</v>
       </c>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="28"/>
+      <c r="Q31" s="28">
+        <v>16297</v>
+      </c>
+      <c r="R31" s="28">
+        <v>16354</v>
+      </c>
+      <c r="S31" s="28">
+        <v>16115</v>
+      </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" s="14"/>
@@ -2352,9 +2406,15 @@
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
+      <c r="Q32" s="25">
+        <v>0</v>
+      </c>
+      <c r="R32" s="25">
+        <v>0</v>
+      </c>
+      <c r="S32" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:19" ht="6.95" customHeight="1">
       <c r="A33" s="14"/>
@@ -2414,9 +2474,15 @@
       <c r="P34" s="28">
         <v>1987144</v>
       </c>
-      <c r="Q34" s="28"/>
-      <c r="R34" s="28"/>
-      <c r="S34" s="28"/>
+      <c r="Q34" s="28">
+        <v>1973548</v>
+      </c>
+      <c r="R34" s="28">
+        <v>1962533</v>
+      </c>
+      <c r="S34" s="28">
+        <v>1983889</v>
+      </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" s="14"/>
@@ -2504,15 +2570,15 @@
       </c>
       <c r="Q37" s="105">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>426464</v>
       </c>
       <c r="R37" s="105">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>417847</v>
       </c>
       <c r="S37" s="105">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>423917</v>
       </c>
     </row>
     <row r="38" spans="1:19" s="37" customFormat="1" ht="14.25" customHeight="1">
@@ -2563,15 +2629,15 @@
       </c>
       <c r="Q38" s="35">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>194026</v>
       </c>
       <c r="R38" s="35">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>189083</v>
       </c>
       <c r="S38" s="35">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>195075</v>
       </c>
     </row>
     <row r="39" spans="1:19" s="29" customFormat="1">
@@ -2611,9 +2677,15 @@
       <c r="P39" s="38">
         <v>232833</v>
       </c>
-      <c r="Q39" s="38"/>
-      <c r="R39" s="38"/>
-      <c r="S39" s="38"/>
+      <c r="Q39" s="38">
+        <v>193890</v>
+      </c>
+      <c r="R39" s="38">
+        <v>188947</v>
+      </c>
+      <c r="S39" s="38">
+        <v>194939</v>
+      </c>
     </row>
     <row r="40" spans="1:19" s="29" customFormat="1" ht="12.75" customHeight="1">
       <c r="A40" s="27"/>
@@ -2652,9 +2724,15 @@
       <c r="P40" s="38">
         <v>136</v>
       </c>
-      <c r="Q40" s="38"/>
-      <c r="R40" s="38"/>
-      <c r="S40" s="38"/>
+      <c r="Q40" s="38">
+        <v>136</v>
+      </c>
+      <c r="R40" s="38">
+        <v>136</v>
+      </c>
+      <c r="S40" s="38">
+        <v>136</v>
+      </c>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="14"/>
@@ -2724,15 +2802,15 @@
       </c>
       <c r="Q42" s="35">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>232438</v>
       </c>
       <c r="R42" s="35">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>228764</v>
       </c>
       <c r="S42" s="35">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>228842</v>
       </c>
     </row>
     <row r="43" spans="1:19" s="40" customFormat="1">
@@ -2766,9 +2844,15 @@
       <c r="P43" s="38">
         <v>195542</v>
       </c>
-      <c r="Q43" s="38"/>
-      <c r="R43" s="38"/>
-      <c r="S43" s="38"/>
+      <c r="Q43" s="38">
+        <v>228113</v>
+      </c>
+      <c r="R43" s="38">
+        <v>224455</v>
+      </c>
+      <c r="S43" s="38">
+        <v>224482</v>
+      </c>
     </row>
     <row r="44" spans="1:19" s="40" customFormat="1" ht="12.75" customHeight="1">
       <c r="E44" s="42" t="s">
@@ -2801,9 +2885,15 @@
       <c r="P44" s="38">
         <v>4352</v>
       </c>
-      <c r="Q44" s="38"/>
-      <c r="R44" s="38"/>
-      <c r="S44" s="38"/>
+      <c r="Q44" s="38">
+        <v>4325</v>
+      </c>
+      <c r="R44" s="38">
+        <v>4309</v>
+      </c>
+      <c r="S44" s="38">
+        <v>4360</v>
+      </c>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="43"/>

</xml_diff>

<commit_message>
Q2 2022 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AD77DD-F581-47ED-A8B9-D216386F0E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8088E456-1810-4088-A139-EA8EA7E0C4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13875" yWindow="2430" windowWidth="12345" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6870" yWindow="3495" windowWidth="18570" windowHeight="10815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="15" r:id="rId1"/>
@@ -1145,7 +1145,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50786131-2AB4-4B56-BC3B-96AAC9C5A935}">
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1301,15 +1303,15 @@
       </c>
       <c r="K8" s="17">
         <f>+K10+K37</f>
-        <v>0</v>
+        <v>13176615</v>
       </c>
       <c r="L8" s="17">
         <f>+L10+L37</f>
-        <v>0</v>
+        <v>12895488</v>
       </c>
       <c r="M8" s="17">
         <f t="shared" ref="M8:S8" si="0">+M10+M37</f>
-        <v>0</v>
+        <v>13205756</v>
       </c>
       <c r="N8" s="17">
         <f t="shared" si="0"/>
@@ -1381,15 +1383,15 @@
       </c>
       <c r="K10" s="101">
         <f>+K12+K27</f>
-        <v>0</v>
+        <v>12763187</v>
       </c>
       <c r="L10" s="101">
         <f>+L12+L27</f>
-        <v>0</v>
+        <v>12495772</v>
       </c>
       <c r="M10" s="101">
         <f t="shared" ref="M10:S10" si="1">+M12+M27</f>
-        <v>0</v>
+        <v>12791829</v>
       </c>
       <c r="N10" s="101">
         <f t="shared" si="1"/>
@@ -1461,15 +1463,15 @@
       </c>
       <c r="K12" s="23">
         <f>+K13+K25</f>
-        <v>0</v>
+        <v>8935854</v>
       </c>
       <c r="L12" s="23">
         <f>+L13+L25</f>
-        <v>0</v>
+        <v>8665450</v>
       </c>
       <c r="M12" s="23">
         <f t="shared" ref="M12:S12" si="2">+M13+M25</f>
-        <v>0</v>
+        <v>8767110</v>
       </c>
       <c r="N12" s="23">
         <f t="shared" si="2"/>
@@ -1520,15 +1522,15 @@
       </c>
       <c r="K13" s="23">
         <f>K14+K19</f>
-        <v>0</v>
+        <v>300156</v>
       </c>
       <c r="L13" s="23">
         <f>L14+L19</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="M13" s="23">
         <f t="shared" ref="M13:S13" si="3">M14+M19</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="N13" s="23">
         <f t="shared" si="3"/>
@@ -1579,15 +1581,15 @@
       </c>
       <c r="K14" s="25">
         <f>K15+K18</f>
-        <v>0</v>
+        <v>300156</v>
       </c>
       <c r="L14" s="25">
         <f>L15+L18</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="M14" s="25">
         <f t="shared" ref="M14:S14" si="4">M15+M18</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="N14" s="25">
         <f t="shared" si="4"/>
@@ -1633,9 +1635,15 @@
       <c r="J15" s="26">
         <v>300156</v>
       </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
+      <c r="K15" s="26">
+        <v>300156</v>
+      </c>
+      <c r="L15" s="26">
+        <v>156</v>
+      </c>
+      <c r="M15" s="26">
+        <v>156</v>
+      </c>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
@@ -1662,9 +1670,15 @@
       <c r="J16" s="26">
         <v>156</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
+      <c r="K16" s="26">
+        <v>156</v>
+      </c>
+      <c r="L16" s="26">
+        <v>156</v>
+      </c>
+      <c r="M16" s="26">
+        <v>156</v>
+      </c>
       <c r="N16" s="26"/>
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
@@ -1691,9 +1705,15 @@
       <c r="J17" s="26">
         <v>300000</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
+      <c r="K17" s="26">
+        <v>300000</v>
+      </c>
+      <c r="L17" s="26">
+        <v>0</v>
+      </c>
+      <c r="M17" s="26">
+        <v>0</v>
+      </c>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
@@ -1720,9 +1740,15 @@
       <c r="J18" s="26">
         <v>0</v>
       </c>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
+      <c r="K18" s="26">
+        <v>0</v>
+      </c>
+      <c r="L18" s="26">
+        <v>0</v>
+      </c>
+      <c r="M18" s="26">
+        <v>0</v>
+      </c>
       <c r="N18" s="26"/>
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
@@ -1741,31 +1767,25 @@
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
       <c r="H19" s="25">
-        <f>SUM(H20:H23)</f>
         <v>0</v>
       </c>
       <c r="I19" s="25">
-        <f>SUM(I20:I23)</f>
         <v>0</v>
       </c>
       <c r="J19" s="25">
-        <f>SUM(J20:J23)</f>
         <v>0</v>
       </c>
       <c r="K19" s="25">
-        <f>SUM(K20:K23)</f>
         <v>0</v>
       </c>
       <c r="L19" s="25">
-        <f>SUM(L20:L23)</f>
         <v>0</v>
       </c>
       <c r="M19" s="25">
-        <f t="shared" ref="M19:S19" si="5">SUM(M20:M23)</f>
         <v>0</v>
       </c>
       <c r="N19" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M19:S19" si="5">SUM(N20:N23)</f>
         <v>0</v>
       </c>
       <c r="O19" s="25">
@@ -1941,9 +1961,15 @@
       <c r="J25" s="28">
         <v>8568495</v>
       </c>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
+      <c r="K25" s="28">
+        <v>8635698</v>
+      </c>
+      <c r="L25" s="28">
+        <v>8665294</v>
+      </c>
+      <c r="M25" s="28">
+        <v>8766954</v>
+      </c>
       <c r="N25" s="28"/>
       <c r="O25" s="28"/>
       <c r="P25" s="28"/>
@@ -1996,15 +2022,15 @@
       </c>
       <c r="K27" s="23">
         <f>K28+K34</f>
-        <v>0</v>
+        <v>3827333</v>
       </c>
       <c r="L27" s="23">
         <f>L28+L34</f>
-        <v>0</v>
+        <v>3830322</v>
       </c>
       <c r="M27" s="23">
         <f t="shared" ref="M27:S27" si="6">M28+M34</f>
-        <v>0</v>
+        <v>4024719</v>
       </c>
       <c r="N27" s="23">
         <f t="shared" si="6"/>
@@ -2055,15 +2081,15 @@
       </c>
       <c r="K28" s="25">
         <f>K29+K32</f>
-        <v>0</v>
+        <v>1675248</v>
       </c>
       <c r="L28" s="25">
         <f>L29+L32</f>
-        <v>0</v>
+        <v>1690029</v>
       </c>
       <c r="M28" s="25">
         <f t="shared" ref="M28:S28" si="7">M29+M32</f>
-        <v>0</v>
+        <v>1795604</v>
       </c>
       <c r="N28" s="25">
         <f t="shared" si="7"/>
@@ -2114,15 +2140,15 @@
       </c>
       <c r="K29" s="30">
         <f>+K30+K31</f>
-        <v>0</v>
+        <v>1675248</v>
       </c>
       <c r="L29" s="30">
         <f>+L30+L31</f>
-        <v>0</v>
+        <v>1690029</v>
       </c>
       <c r="M29" s="30">
         <f t="shared" ref="M29:S29" si="8">+M30+M31</f>
-        <v>0</v>
+        <v>1795604</v>
       </c>
       <c r="N29" s="30">
         <f t="shared" si="8"/>
@@ -2168,9 +2194,15 @@
       <c r="J30" s="28">
         <v>1671980</v>
       </c>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
+      <c r="K30" s="28">
+        <v>1661314</v>
+      </c>
+      <c r="L30" s="28">
+        <v>1675941</v>
+      </c>
+      <c r="M30" s="28">
+        <v>1781701</v>
+      </c>
       <c r="N30" s="28"/>
       <c r="O30" s="28"/>
       <c r="P30" s="28"/>
@@ -2197,9 +2229,15 @@
       <c r="J31" s="28">
         <v>14950</v>
       </c>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
+      <c r="K31" s="28">
+        <v>13934</v>
+      </c>
+      <c r="L31" s="28">
+        <v>14088</v>
+      </c>
+      <c r="M31" s="28">
+        <v>13903</v>
+      </c>
       <c r="N31" s="28"/>
       <c r="O31" s="28"/>
       <c r="P31" s="28"/>
@@ -2226,9 +2264,15 @@
       <c r="J32" s="25">
         <v>0</v>
       </c>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
+      <c r="K32" s="25">
+        <v>0</v>
+      </c>
+      <c r="L32" s="25">
+        <v>0</v>
+      </c>
+      <c r="M32" s="25">
+        <v>0</v>
+      </c>
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -2276,9 +2320,15 @@
       <c r="J34" s="28">
         <v>2124204</v>
       </c>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
+      <c r="K34" s="28">
+        <v>2152085</v>
+      </c>
+      <c r="L34" s="28">
+        <v>2140293</v>
+      </c>
+      <c r="M34" s="28">
+        <v>2229115</v>
+      </c>
       <c r="N34" s="28"/>
       <c r="O34" s="28"/>
       <c r="P34" s="28"/>
@@ -2348,15 +2398,15 @@
       </c>
       <c r="K37" s="105">
         <f>+K38+K42</f>
-        <v>0</v>
+        <v>413428</v>
       </c>
       <c r="L37" s="105">
         <f>+L38+L42</f>
-        <v>0</v>
+        <v>399716</v>
       </c>
       <c r="M37" s="105">
         <f t="shared" ref="M37:S37" si="9">+M38+M42</f>
-        <v>0</v>
+        <v>413927</v>
       </c>
       <c r="N37" s="105">
         <f t="shared" si="9"/>
@@ -2407,15 +2457,15 @@
       </c>
       <c r="K38" s="35">
         <f>+K39+K40</f>
-        <v>0</v>
+        <v>194292</v>
       </c>
       <c r="L38" s="35">
         <f>+L39+L40</f>
-        <v>0</v>
+        <v>185885</v>
       </c>
       <c r="M38" s="35">
         <f t="shared" ref="M38:S38" si="10">+M39+M40</f>
-        <v>0</v>
+        <v>195224</v>
       </c>
       <c r="N38" s="35">
         <f t="shared" si="10"/>
@@ -2461,9 +2511,15 @@
       <c r="J39" s="38">
         <v>187999</v>
       </c>
-      <c r="K39" s="38"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="38"/>
+      <c r="K39" s="38">
+        <v>194156</v>
+      </c>
+      <c r="L39" s="38">
+        <v>185749</v>
+      </c>
+      <c r="M39" s="38">
+        <v>195088</v>
+      </c>
       <c r="N39" s="38"/>
       <c r="O39" s="38"/>
       <c r="P39" s="38"/>
@@ -2490,9 +2546,15 @@
       <c r="J40" s="38">
         <v>136</v>
       </c>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="38"/>
+      <c r="K40" s="38">
+        <v>136</v>
+      </c>
+      <c r="L40" s="38">
+        <v>136</v>
+      </c>
+      <c r="M40" s="38">
+        <v>136</v>
+      </c>
       <c r="N40" s="38"/>
       <c r="O40" s="38"/>
       <c r="P40" s="38"/>
@@ -2544,15 +2606,15 @@
       </c>
       <c r="K42" s="35">
         <f>+K43+K44</f>
-        <v>0</v>
+        <v>219136</v>
       </c>
       <c r="L42" s="35">
         <f>+L43+L44</f>
-        <v>0</v>
+        <v>213831</v>
       </c>
       <c r="M42" s="35">
         <f t="shared" ref="M42:S42" si="11">+M43+M44</f>
-        <v>0</v>
+        <v>218703</v>
       </c>
       <c r="N42" s="35">
         <f t="shared" si="11"/>
@@ -2592,9 +2654,15 @@
       <c r="J43" s="38">
         <v>218470</v>
       </c>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
+      <c r="K43" s="38">
+        <v>214661</v>
+      </c>
+      <c r="L43" s="38">
+        <v>209349</v>
+      </c>
+      <c r="M43" s="38">
+        <v>214003</v>
+      </c>
       <c r="N43" s="38"/>
       <c r="O43" s="38"/>
       <c r="P43" s="38"/>
@@ -2615,9 +2683,15 @@
       <c r="J44" s="38">
         <v>4439</v>
       </c>
-      <c r="K44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
+      <c r="K44" s="38">
+        <v>4475</v>
+      </c>
+      <c r="L44" s="38">
+        <v>4482</v>
+      </c>
+      <c r="M44" s="38">
+        <v>4700</v>
+      </c>
       <c r="N44" s="38"/>
       <c r="O44" s="38"/>
       <c r="P44" s="38"/>
@@ -13327,7 +13401,7 @@
   <dimension ref="A1:S189"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Q3 2024 Fiscal Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03738C3-32D6-47C5-B6DB-99FD63DD49E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA2D1D3-DD1C-4A7B-B2C8-BCC343FF905F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="3840" windowWidth="11145" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="16" r:id="rId1"/>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:S189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1194,15 +1194,15 @@
       </c>
       <c r="N8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16034777</v>
       </c>
       <c r="O8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15914225</v>
       </c>
       <c r="P8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16266167</v>
       </c>
       <c r="Q8" s="16">
         <f t="shared" si="0"/>
@@ -1266,15 +1266,15 @@
       </c>
       <c r="N10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15689987</v>
       </c>
       <c r="O10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15550200</v>
       </c>
       <c r="P10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15893305</v>
       </c>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
@@ -1343,15 +1343,15 @@
       </c>
       <c r="N12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10753150</v>
       </c>
       <c r="O12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10791608</v>
       </c>
       <c r="P12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10936258</v>
       </c>
       <c r="Q12" s="20">
         <f t="shared" si="2"/>
@@ -1400,15 +1400,15 @@
       </c>
       <c r="N13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="O13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="P13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="Q13" s="20">
         <f t="shared" si="3"/>
@@ -1457,15 +1457,15 @@
       </c>
       <c r="N14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="O14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="P14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="Q14" s="22">
         <f t="shared" si="4"/>
@@ -1506,9 +1506,15 @@
       <c r="M15" s="23">
         <v>156</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
+      <c r="N15" s="23">
+        <v>156</v>
+      </c>
+      <c r="O15" s="23">
+        <v>156</v>
+      </c>
+      <c r="P15" s="23">
+        <v>156</v>
+      </c>
       <c r="Q15" s="23"/>
       <c r="R15" s="23"/>
       <c r="S15" s="23"/>
@@ -1539,9 +1545,15 @@
       <c r="M16" s="23">
         <v>156</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
+      <c r="N16" s="23">
+        <v>156</v>
+      </c>
+      <c r="O16" s="23">
+        <v>156</v>
+      </c>
+      <c r="P16" s="23">
+        <v>156</v>
+      </c>
       <c r="Q16" s="23"/>
       <c r="R16" s="23"/>
       <c r="S16" s="23"/>
@@ -1878,9 +1890,15 @@
       <c r="M25" s="25">
         <v>10572960</v>
       </c>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
+      <c r="N25" s="25">
+        <v>10752994</v>
+      </c>
+      <c r="O25" s="25">
+        <v>10791452</v>
+      </c>
+      <c r="P25" s="25">
+        <v>10936102</v>
+      </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
@@ -1938,15 +1956,15 @@
       </c>
       <c r="N27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4936837</v>
       </c>
       <c r="O27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4758592</v>
       </c>
       <c r="P27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4957047</v>
       </c>
       <c r="Q27" s="20">
         <f t="shared" si="5"/>
@@ -1995,15 +2013,15 @@
       </c>
       <c r="N28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2320010</v>
       </c>
       <c r="O28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2245024</v>
       </c>
       <c r="P28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2318595</v>
       </c>
       <c r="Q28" s="22">
         <f t="shared" si="6"/>
@@ -2052,15 +2070,15 @@
       </c>
       <c r="N29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2320010</v>
       </c>
       <c r="O29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2245024</v>
       </c>
       <c r="P29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2318595</v>
       </c>
       <c r="Q29" s="26">
         <f t="shared" si="7"/>
@@ -2101,9 +2119,15 @@
       <c r="M30" s="25">
         <v>2282825</v>
       </c>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
+      <c r="N30" s="25">
+        <v>2309746</v>
+      </c>
+      <c r="O30" s="25">
+        <v>2234914</v>
+      </c>
+      <c r="P30" s="25">
+        <v>2308672</v>
+      </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -2134,9 +2158,15 @@
       <c r="M31" s="25">
         <v>9618</v>
       </c>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
+      <c r="N31" s="25">
+        <v>10264</v>
+      </c>
+      <c r="O31" s="25">
+        <v>10110</v>
+      </c>
+      <c r="P31" s="25">
+        <v>9923</v>
+      </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
@@ -2231,9 +2261,15 @@
       <c r="M34" s="25">
         <v>2617940</v>
       </c>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
+      <c r="N34" s="25">
+        <v>2616827</v>
+      </c>
+      <c r="O34" s="25">
+        <v>2513568</v>
+      </c>
+      <c r="P34" s="25">
+        <v>2638452</v>
+      </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
@@ -2293,15 +2329,15 @@
       </c>
       <c r="N37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>344790</v>
       </c>
       <c r="O37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>364025</v>
       </c>
       <c r="P37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>372862</v>
       </c>
       <c r="Q37" s="32">
         <f t="shared" si="8"/>
@@ -2346,15 +2382,15 @@
       </c>
       <c r="N38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>180859</v>
       </c>
       <c r="O38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>205158</v>
       </c>
       <c r="P38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>214958</v>
       </c>
       <c r="Q38" s="34">
         <f t="shared" si="9"/>
@@ -2391,9 +2427,15 @@
       <c r="M39" s="35">
         <v>182435</v>
       </c>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
+      <c r="N39" s="35">
+        <v>180723</v>
+      </c>
+      <c r="O39" s="35">
+        <v>205022</v>
+      </c>
+      <c r="P39" s="35">
+        <v>214822</v>
+      </c>
       <c r="Q39" s="35"/>
       <c r="R39" s="35"/>
       <c r="S39" s="35"/>
@@ -2420,9 +2462,15 @@
       <c r="M40" s="35">
         <v>136</v>
       </c>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
+      <c r="N40" s="35">
+        <v>136</v>
+      </c>
+      <c r="O40" s="35">
+        <v>136</v>
+      </c>
+      <c r="P40" s="35">
+        <v>136</v>
+      </c>
       <c r="Q40" s="35"/>
       <c r="R40" s="35"/>
       <c r="S40" s="35"/>
@@ -2474,15 +2522,15 @@
       </c>
       <c r="N42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>163931</v>
       </c>
       <c r="O42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>158867</v>
       </c>
       <c r="P42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>157904</v>
       </c>
       <c r="Q42" s="34">
         <f t="shared" si="9"/>
@@ -2519,6 +2567,15 @@
       <c r="M43" s="35">
         <v>156061</v>
       </c>
+      <c r="N43" s="35">
+        <v>158931</v>
+      </c>
+      <c r="O43" s="35">
+        <v>154064</v>
+      </c>
+      <c r="P43" s="35">
+        <v>153114</v>
+      </c>
     </row>
     <row r="44" spans="1:19" s="35" customFormat="1" ht="12.75" customHeight="1">
       <c r="E44" s="35" t="s">
@@ -2541,6 +2598,15 @@
       </c>
       <c r="M44" s="35">
         <v>5015</v>
+      </c>
+      <c r="N44" s="35">
+        <v>5000</v>
+      </c>
+      <c r="O44" s="35">
+        <v>4803</v>
+      </c>
+      <c r="P44" s="35">
+        <v>4790</v>
       </c>
     </row>
     <row r="47" spans="1:19">

</xml_diff>

<commit_message>
Q4 2024 Fiscal Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA2D1D3-DD1C-4A7B-B2C8-BCC343FF905F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA0449E-732F-49CE-A2B8-46B0B9A9C47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="16" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="77">
   <si>
     <t xml:space="preserve">National Government Outstanding Debt Stock </t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>CY 2009</t>
+  </si>
+  <si>
+    <t>CY 2024</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4D0018-5634-44D5-B16B-720E758CF0F4}">
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1092,7 +1095,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="78" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="79"/>
@@ -1206,15 +1209,15 @@
       </c>
       <c r="Q8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16432017</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16513000</v>
       </c>
       <c r="S8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16397961</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="14" customFormat="1">
@@ -1278,15 +1281,15 @@
       </c>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16020258</v>
       </c>
       <c r="R10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16090966</v>
       </c>
       <c r="S10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16051302</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="6.95" customHeight="1">
@@ -1355,15 +1358,15 @@
       </c>
       <c r="Q12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10889837</v>
       </c>
       <c r="R12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10921662</v>
       </c>
       <c r="S12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10930415</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1412,15 +1415,15 @@
       </c>
       <c r="Q13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="R13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="S13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1469,15 +1472,15 @@
       </c>
       <c r="Q14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="R14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="S14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1515,9 +1518,15 @@
       <c r="P15" s="23">
         <v>156</v>
       </c>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
+      <c r="Q15" s="23">
+        <v>156</v>
+      </c>
+      <c r="R15" s="23">
+        <v>156</v>
+      </c>
+      <c r="S15" s="23">
+        <v>156</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="C16" s="21"/>
@@ -1554,9 +1563,15 @@
       <c r="P16" s="23">
         <v>156</v>
       </c>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
+      <c r="Q16" s="23">
+        <v>156</v>
+      </c>
+      <c r="R16" s="23">
+        <v>156</v>
+      </c>
+      <c r="S16" s="23">
+        <v>156</v>
+      </c>
     </row>
     <row r="17" spans="3:19">
       <c r="C17" s="21"/>
@@ -1899,9 +1914,15 @@
       <c r="P25" s="25">
         <v>10936102</v>
       </c>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
+      <c r="Q25" s="25">
+        <v>10889681</v>
+      </c>
+      <c r="R25" s="25">
+        <v>10921506</v>
+      </c>
+      <c r="S25" s="25">
+        <v>10930259</v>
+      </c>
     </row>
     <row r="26" spans="3:19">
       <c r="C26" s="21"/>
@@ -1968,15 +1989,15 @@
       </c>
       <c r="Q27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5130421</v>
       </c>
       <c r="R27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5169304</v>
       </c>
       <c r="S27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5120887</v>
       </c>
     </row>
     <row r="28" spans="3:19" s="24" customFormat="1">
@@ -2025,15 +2046,15 @@
       </c>
       <c r="Q28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2420218</v>
       </c>
       <c r="R28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2445960</v>
       </c>
       <c r="S28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2438865</v>
       </c>
     </row>
     <row r="29" spans="3:19">
@@ -2082,15 +2103,15 @@
       </c>
       <c r="Q29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2420218</v>
       </c>
       <c r="R29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2445960</v>
       </c>
       <c r="S29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2438865</v>
       </c>
     </row>
     <row r="30" spans="3:19">
@@ -2128,9 +2149,15 @@
       <c r="P30" s="25">
         <v>2308672</v>
       </c>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
+      <c r="Q30" s="25">
+        <v>2410665</v>
+      </c>
+      <c r="R30" s="25">
+        <v>2436188</v>
+      </c>
+      <c r="S30" s="25">
+        <v>2429789</v>
+      </c>
     </row>
     <row r="31" spans="3:19">
       <c r="C31" s="21"/>
@@ -2167,9 +2194,15 @@
       <c r="P31" s="25">
         <v>9923</v>
       </c>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
+      <c r="Q31" s="25">
+        <v>9553</v>
+      </c>
+      <c r="R31" s="25">
+        <v>9772</v>
+      </c>
+      <c r="S31" s="25">
+        <v>9076</v>
+      </c>
     </row>
     <row r="32" spans="3:19">
       <c r="C32" s="21"/>
@@ -2270,9 +2303,15 @@
       <c r="P34" s="25">
         <v>2638452</v>
       </c>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
-      <c r="S34" s="25"/>
+      <c r="Q34" s="25">
+        <v>2710203</v>
+      </c>
+      <c r="R34" s="25">
+        <v>2723344</v>
+      </c>
+      <c r="S34" s="25">
+        <v>2682022</v>
+      </c>
     </row>
     <row r="35" spans="1:19">
       <c r="C35" s="19"/>
@@ -2341,15 +2380,15 @@
       </c>
       <c r="Q37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>411759</v>
       </c>
       <c r="R37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>422034</v>
       </c>
       <c r="S37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>346659</v>
       </c>
     </row>
     <row r="38" spans="1:19" s="33" customFormat="1" ht="14.25" customHeight="1">
@@ -2394,15 +2433,15 @@
       </c>
       <c r="Q38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>250807</v>
       </c>
       <c r="R38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>259756</v>
       </c>
       <c r="S38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>255506</v>
       </c>
     </row>
     <row r="39" spans="1:19" s="24" customFormat="1">
@@ -2436,9 +2475,15 @@
       <c r="P39" s="35">
         <v>214822</v>
       </c>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
-      <c r="S39" s="35"/>
+      <c r="Q39" s="35">
+        <v>250671</v>
+      </c>
+      <c r="R39" s="35">
+        <v>259620</v>
+      </c>
+      <c r="S39" s="35">
+        <v>255370</v>
+      </c>
     </row>
     <row r="40" spans="1:19" s="24" customFormat="1" ht="12.75" customHeight="1">
       <c r="E40" s="24" t="s">
@@ -2471,9 +2516,15 @@
       <c r="P40" s="35">
         <v>136</v>
       </c>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
+      <c r="Q40" s="35">
+        <v>136</v>
+      </c>
+      <c r="R40" s="35">
+        <v>136</v>
+      </c>
+      <c r="S40" s="35">
+        <v>136</v>
+      </c>
     </row>
     <row r="41" spans="1:19">
       <c r="E41" s="14"/>
@@ -2534,15 +2585,15 @@
       </c>
       <c r="Q42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>160952</v>
       </c>
       <c r="R42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>162278</v>
       </c>
       <c r="S42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>91153</v>
       </c>
     </row>
     <row r="43" spans="1:19" s="35" customFormat="1">
@@ -2576,6 +2627,15 @@
       <c r="P43" s="35">
         <v>153114</v>
       </c>
+      <c r="Q43" s="35">
+        <v>155977</v>
+      </c>
+      <c r="R43" s="35">
+        <v>157269</v>
+      </c>
+      <c r="S43" s="35">
+        <v>86210</v>
+      </c>
     </row>
     <row r="44" spans="1:19" s="35" customFormat="1" ht="12.75" customHeight="1">
       <c r="E44" s="35" t="s">
@@ -2607,6 +2667,15 @@
       </c>
       <c r="P44" s="35">
         <v>4790</v>
+      </c>
+      <c r="Q44" s="35">
+        <v>4975</v>
+      </c>
+      <c r="R44" s="35">
+        <v>5009</v>
+      </c>
+      <c r="S44" s="35">
+        <v>4943</v>
       </c>
     </row>
     <row r="47" spans="1:19">

</xml_diff>

<commit_message>
Q2 2025 Fiscal Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2059A03E-7C7A-4A3B-83FF-C77256301804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF76AD3-AA1D-476F-A8EF-AFCD24681BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="1905" windowWidth="15270" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="17" r:id="rId1"/>
@@ -313,11 +313,18 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -471,6 +478,11 @@
       <i/>
       <sz val="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -642,175 +654,179 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="37" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="38" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="38" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="37" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="37" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="37" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="38" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="37" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{19C30A91-F072-4922-A132-42DEAD7F215A}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{CC0D16C9-9BB4-4E07-AF9D-1803D9292C33}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1037,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3273FFF-38CF-4648-BAF5-82868DEFDB4E}">
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1178,7 +1194,7 @@
       <c r="G8" s="81"/>
       <c r="H8" s="16">
         <f>+H10+H37</f>
-        <v>16659042.630000001</v>
+        <v>16659043</v>
       </c>
       <c r="I8" s="16">
         <f>+I10+I37</f>
@@ -1194,11 +1210,11 @@
       </c>
       <c r="L8" s="16">
         <f>+L10+L37</f>
-        <v>0</v>
+        <v>17262457</v>
       </c>
       <c r="M8" s="16">
         <f t="shared" ref="M8:S8" si="0">+M10+M37</f>
-        <v>0</v>
+        <v>17612435</v>
       </c>
       <c r="N8" s="16">
         <f t="shared" si="0"/>
@@ -1250,7 +1266,7 @@
       <c r="G10" s="82"/>
       <c r="H10" s="17">
         <f>+H12+H27</f>
-        <v>16312771.630000001</v>
+        <v>16312772</v>
       </c>
       <c r="I10" s="17">
         <f>+I12+I27</f>
@@ -1266,11 +1282,11 @@
       </c>
       <c r="L10" s="17">
         <f>+L12+L27</f>
-        <v>0</v>
+        <v>16918881</v>
       </c>
       <c r="M10" s="17">
         <f t="shared" ref="M10:S10" si="1">+M12+M27</f>
-        <v>0</v>
+        <v>17267328</v>
       </c>
       <c r="N10" s="17">
         <f t="shared" si="1"/>
@@ -1327,7 +1343,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="20">
         <f>+H13+H25</f>
-        <v>11084089.630000001</v>
+        <v>11084090</v>
       </c>
       <c r="I12" s="20">
         <f>+I13+I25</f>
@@ -1343,11 +1359,11 @@
       </c>
       <c r="L12" s="20">
         <f>+L13+L25</f>
-        <v>0</v>
+        <v>11780519</v>
       </c>
       <c r="M12" s="20">
         <f t="shared" ref="M12:S12" si="2">+M13+M25</f>
-        <v>0</v>
+        <v>11950406</v>
       </c>
       <c r="N12" s="20">
         <f t="shared" si="2"/>
@@ -1400,11 +1416,11 @@
       </c>
       <c r="L13" s="20">
         <f>L14+L19</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="M13" s="20">
         <f t="shared" ref="M13:S13" si="3">M14+M19</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="N13" s="20">
         <f t="shared" si="3"/>
@@ -1457,11 +1473,11 @@
       </c>
       <c r="L14" s="22">
         <f>L15+L18</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="M14" s="22">
         <f t="shared" ref="M14:S14" si="4">M15+M18</f>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="N14" s="22">
         <f t="shared" si="4"/>
@@ -1508,8 +1524,12 @@
       <c r="K15" s="23">
         <v>156</v>
       </c>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
+      <c r="L15" s="23">
+        <v>156</v>
+      </c>
+      <c r="M15" s="23">
+        <v>156</v>
+      </c>
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
@@ -1537,8 +1557,12 @@
       <c r="K16" s="23">
         <v>156</v>
       </c>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
+      <c r="L16" s="23">
+        <v>156</v>
+      </c>
+      <c r="M16" s="23">
+        <v>156</v>
+      </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
@@ -1566,8 +1590,12 @@
       <c r="K17" s="23">
         <v>0</v>
       </c>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
+      <c r="L17" s="23">
+        <v>0</v>
+      </c>
+      <c r="M17" s="23">
+        <v>0</v>
+      </c>
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
@@ -1595,8 +1623,12 @@
       <c r="K18" s="23">
         <v>0</v>
       </c>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
+      <c r="L18" s="23">
+        <v>0</v>
+      </c>
+      <c r="M18" s="23">
+        <v>0</v>
+      </c>
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
@@ -1624,8 +1656,12 @@
       <c r="K19" s="22">
         <v>0</v>
       </c>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
+      <c r="L19" s="22">
+        <v>0</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0</v>
+      </c>
       <c r="N19" s="22"/>
       <c r="O19" s="22"/>
       <c r="P19" s="22"/>
@@ -1765,7 +1801,7 @@
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="25">
-        <v>11083933.630000001</v>
+        <v>11083934</v>
       </c>
       <c r="I25" s="25">
         <v>11223553</v>
@@ -1776,8 +1812,12 @@
       <c r="K25" s="25">
         <v>11590402</v>
       </c>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
+      <c r="L25" s="25">
+        <v>11780363</v>
+      </c>
+      <c r="M25" s="25">
+        <v>11950250</v>
+      </c>
       <c r="N25" s="25"/>
       <c r="O25" s="25"/>
       <c r="P25" s="25"/>
@@ -1830,11 +1870,11 @@
       </c>
       <c r="L27" s="20">
         <f>L28+L34</f>
-        <v>0</v>
+        <v>5138362</v>
       </c>
       <c r="M27" s="20">
         <f t="shared" ref="M27:S27" si="5">M28+M34</f>
-        <v>0</v>
+        <v>5316922</v>
       </c>
       <c r="N27" s="20">
         <f t="shared" si="5"/>
@@ -1887,11 +1927,11 @@
       </c>
       <c r="L28" s="22">
         <f>L29+L32</f>
-        <v>0</v>
+        <v>2468786</v>
       </c>
       <c r="M28" s="22">
         <f t="shared" ref="M28:S28" si="6">M29+M32</f>
-        <v>0</v>
+        <v>2602397</v>
       </c>
       <c r="N28" s="22">
         <f t="shared" si="6"/>
@@ -1944,11 +1984,11 @@
       </c>
       <c r="L29" s="26">
         <f>+L30+L31</f>
-        <v>0</v>
+        <v>2468786</v>
       </c>
       <c r="M29" s="26">
         <f t="shared" ref="M29:S29" si="7">+M30+M31</f>
-        <v>0</v>
+        <v>2602397</v>
       </c>
       <c r="N29" s="26">
         <f t="shared" si="7"/>
@@ -1995,8 +2035,12 @@
       <c r="K30" s="25">
         <v>2470606</v>
       </c>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
+      <c r="L30" s="25">
+        <v>2459779</v>
+      </c>
+      <c r="M30" s="25">
+        <v>2593272</v>
+      </c>
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
@@ -2024,8 +2068,12 @@
       <c r="K31" s="25">
         <v>8967</v>
       </c>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
+      <c r="L31" s="25">
+        <v>9007</v>
+      </c>
+      <c r="M31" s="25">
+        <v>9125</v>
+      </c>
       <c r="N31" s="25"/>
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
@@ -2053,8 +2101,12 @@
       <c r="K32" s="22">
         <v>0</v>
       </c>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
+      <c r="L32" s="22">
+        <v>0</v>
+      </c>
+      <c r="M32" s="22">
+        <v>0</v>
+      </c>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
@@ -2101,8 +2153,12 @@
       <c r="K34" s="25">
         <v>2682544</v>
       </c>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
+      <c r="L34" s="25">
+        <v>2669576</v>
+      </c>
+      <c r="M34" s="25">
+        <v>2714525</v>
+      </c>
       <c r="N34" s="25"/>
       <c r="O34" s="25"/>
       <c r="P34" s="25"/>
@@ -2157,11 +2213,11 @@
       </c>
       <c r="L37" s="32">
         <f>+L38+L42</f>
-        <v>0</v>
+        <v>343576</v>
       </c>
       <c r="M37" s="32">
         <f t="shared" ref="M37:S37" si="8">+M38+M42</f>
-        <v>0</v>
+        <v>345107</v>
       </c>
       <c r="N37" s="32">
         <f t="shared" si="8"/>
@@ -2210,11 +2266,11 @@
       </c>
       <c r="L38" s="34">
         <f>+L39+L40</f>
-        <v>0</v>
+        <v>253675</v>
       </c>
       <c r="M38" s="34">
         <f t="shared" ref="M38:S42" si="9">+M39+M40</f>
-        <v>0</v>
+        <v>254472</v>
       </c>
       <c r="N38" s="34">
         <f t="shared" si="9"/>
@@ -2257,8 +2313,12 @@
       <c r="K39" s="35">
         <v>247011</v>
       </c>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
+      <c r="L39" s="35">
+        <v>253539</v>
+      </c>
+      <c r="M39" s="35">
+        <v>254336</v>
+      </c>
       <c r="N39" s="35"/>
       <c r="O39" s="35"/>
       <c r="P39" s="35"/>
@@ -2282,8 +2342,12 @@
       <c r="K40" s="35">
         <v>136</v>
       </c>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
+      <c r="L40" s="35">
+        <v>136</v>
+      </c>
+      <c r="M40" s="35">
+        <v>136</v>
+      </c>
       <c r="N40" s="35"/>
       <c r="O40" s="35"/>
       <c r="P40" s="35"/>
@@ -2330,11 +2394,11 @@
       </c>
       <c r="L42" s="34">
         <f>+L43+L44</f>
-        <v>0</v>
+        <v>89901</v>
       </c>
       <c r="M42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>90635</v>
       </c>
       <c r="N42" s="34">
         <f t="shared" si="9"/>
@@ -2377,6 +2441,12 @@
       <c r="K43" s="35">
         <v>85610</v>
       </c>
+      <c r="L43" s="35">
+        <v>85145</v>
+      </c>
+      <c r="M43" s="35">
+        <v>85813</v>
+      </c>
     </row>
     <row r="44" spans="1:19" s="35" customFormat="1" ht="12.75" customHeight="1">
       <c r="E44" s="35" t="s">
@@ -2393,6 +2463,12 @@
       </c>
       <c r="K44" s="35">
         <v>4783</v>
+      </c>
+      <c r="L44" s="35">
+        <v>4756</v>
+      </c>
+      <c r="M44" s="35">
+        <v>4822</v>
       </c>
     </row>
     <row r="47" spans="1:19">

</xml_diff>

<commit_message>
Q3 2025 Fiscal Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF76AD3-AA1D-476F-A8EF-AFCD24681BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F5817F-ADCD-41C9-BB61-A965D01458E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="1890" windowWidth="14715" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="17" r:id="rId1"/>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:S189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1194,7 +1194,7 @@
       <c r="G8" s="81"/>
       <c r="H8" s="16">
         <f>+H10+H37</f>
-        <v>16659043</v>
+        <v>16659042.630000001</v>
       </c>
       <c r="I8" s="16">
         <f>+I10+I37</f>
@@ -1214,19 +1214,19 @@
       </c>
       <c r="M8" s="16">
         <f t="shared" ref="M8:S8" si="0">+M10+M37</f>
-        <v>17612435</v>
+        <v>17612435.009999998</v>
       </c>
       <c r="N8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17916491</v>
       </c>
       <c r="O8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17814905</v>
       </c>
       <c r="P8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17801987</v>
       </c>
       <c r="Q8" s="16">
         <f t="shared" si="0"/>
@@ -1266,7 +1266,7 @@
       <c r="G10" s="82"/>
       <c r="H10" s="17">
         <f>+H12+H27</f>
-        <v>16312772</v>
+        <v>16312771.630000001</v>
       </c>
       <c r="I10" s="17">
         <f>+I12+I27</f>
@@ -1286,19 +1286,19 @@
       </c>
       <c r="M10" s="17">
         <f t="shared" ref="M10:S10" si="1">+M12+M27</f>
-        <v>17267328</v>
+        <v>17267328.009999998</v>
       </c>
       <c r="N10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17563521</v>
       </c>
       <c r="O10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17468448</v>
       </c>
       <c r="P10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17455359</v>
       </c>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
@@ -1343,7 +1343,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="20">
         <f>+H13+H25</f>
-        <v>11084090</v>
+        <v>11084089.630000001</v>
       </c>
       <c r="I12" s="20">
         <f>+I13+I25</f>
@@ -1367,15 +1367,15 @@
       </c>
       <c r="N12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12108421</v>
       </c>
       <c r="O12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12087031</v>
       </c>
       <c r="P12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11972900</v>
       </c>
       <c r="Q12" s="20">
         <f t="shared" si="2"/>
@@ -1424,15 +1424,15 @@
       </c>
       <c r="N13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="O13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="P13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="Q13" s="20">
         <f t="shared" si="3"/>
@@ -1481,15 +1481,15 @@
       </c>
       <c r="N14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="O14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="P14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="Q14" s="22">
         <f t="shared" si="4"/>
@@ -1530,9 +1530,15 @@
       <c r="M15" s="23">
         <v>156</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
+      <c r="N15" s="23">
+        <v>156</v>
+      </c>
+      <c r="O15" s="23">
+        <v>156</v>
+      </c>
+      <c r="P15" s="23">
+        <v>156</v>
+      </c>
       <c r="Q15" s="23"/>
       <c r="R15" s="23"/>
       <c r="S15" s="23"/>
@@ -1563,9 +1569,15 @@
       <c r="M16" s="23">
         <v>156</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
+      <c r="N16" s="23">
+        <v>156</v>
+      </c>
+      <c r="O16" s="23">
+        <v>156</v>
+      </c>
+      <c r="P16" s="23">
+        <v>156</v>
+      </c>
       <c r="Q16" s="23"/>
       <c r="R16" s="23"/>
       <c r="S16" s="23"/>
@@ -1596,9 +1608,15 @@
       <c r="M17" s="23">
         <v>0</v>
       </c>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
+      <c r="N17" s="23">
+        <v>0</v>
+      </c>
+      <c r="O17" s="23">
+        <v>0</v>
+      </c>
+      <c r="P17" s="23">
+        <v>0</v>
+      </c>
       <c r="Q17" s="23"/>
       <c r="R17" s="23"/>
       <c r="S17" s="23"/>
@@ -1629,9 +1647,15 @@
       <c r="M18" s="23">
         <v>0</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
+      <c r="N18" s="23">
+        <v>0</v>
+      </c>
+      <c r="O18" s="23">
+        <v>0</v>
+      </c>
+      <c r="P18" s="23">
+        <v>0</v>
+      </c>
       <c r="Q18" s="23"/>
       <c r="R18" s="23"/>
       <c r="S18" s="23"/>
@@ -1662,9 +1686,15 @@
       <c r="M19" s="22">
         <v>0</v>
       </c>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
+      <c r="N19" s="22">
+        <v>0</v>
+      </c>
+      <c r="O19" s="22">
+        <v>0</v>
+      </c>
+      <c r="P19" s="22">
+        <v>0</v>
+      </c>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
@@ -1801,7 +1831,7 @@
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="25">
-        <v>11083934</v>
+        <v>11083933.630000001</v>
       </c>
       <c r="I25" s="25">
         <v>11223553</v>
@@ -1818,9 +1848,15 @@
       <c r="M25" s="25">
         <v>11950250</v>
       </c>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
+      <c r="N25" s="25">
+        <v>12108265</v>
+      </c>
+      <c r="O25" s="25">
+        <v>12086875</v>
+      </c>
+      <c r="P25" s="25">
+        <v>11972744</v>
+      </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
@@ -1874,19 +1910,19 @@
       </c>
       <c r="M27" s="20">
         <f t="shared" ref="M27:S27" si="5">M28+M34</f>
-        <v>5316922</v>
+        <v>5316922.01</v>
       </c>
       <c r="N27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5455100</v>
       </c>
       <c r="O27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5381417</v>
       </c>
       <c r="P27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5482459</v>
       </c>
       <c r="Q27" s="20">
         <f t="shared" si="5"/>
@@ -1931,19 +1967,19 @@
       </c>
       <c r="M28" s="22">
         <f t="shared" ref="M28:S28" si="6">M29+M32</f>
-        <v>2602397</v>
+        <v>2602397.4</v>
       </c>
       <c r="N28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2666074</v>
       </c>
       <c r="O28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2638810</v>
       </c>
       <c r="P28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2686973</v>
       </c>
       <c r="Q28" s="22">
         <f t="shared" si="6"/>
@@ -1988,19 +2024,19 @@
       </c>
       <c r="M29" s="26">
         <f t="shared" ref="M29:S29" si="7">+M30+M31</f>
-        <v>2602397</v>
+        <v>2602397.4</v>
       </c>
       <c r="N29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2666074</v>
       </c>
       <c r="O29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2638810</v>
       </c>
       <c r="P29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2686973</v>
       </c>
       <c r="Q29" s="26">
         <f t="shared" si="7"/>
@@ -2041,9 +2077,15 @@
       <c r="M30" s="25">
         <v>2593272</v>
       </c>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
+      <c r="N30" s="25">
+        <v>2657082</v>
+      </c>
+      <c r="O30" s="25">
+        <v>2629773</v>
+      </c>
+      <c r="P30" s="25">
+        <v>2678149</v>
+      </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -2072,11 +2114,17 @@
         <v>9007</v>
       </c>
       <c r="M31" s="25">
-        <v>9125</v>
-      </c>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
+        <v>9125.4</v>
+      </c>
+      <c r="N31" s="25">
+        <v>8992</v>
+      </c>
+      <c r="O31" s="25">
+        <v>9037</v>
+      </c>
+      <c r="P31" s="25">
+        <v>8824</v>
+      </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
@@ -2107,9 +2155,15 @@
       <c r="M32" s="22">
         <v>0</v>
       </c>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
+      <c r="N32" s="22">
+        <v>0</v>
+      </c>
+      <c r="O32" s="22">
+        <v>0</v>
+      </c>
+      <c r="P32" s="22">
+        <v>0</v>
+      </c>
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
@@ -2157,11 +2211,17 @@
         <v>2669576</v>
       </c>
       <c r="M34" s="25">
-        <v>2714525</v>
-      </c>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
+        <v>2714524.61</v>
+      </c>
+      <c r="N34" s="25">
+        <v>2789026</v>
+      </c>
+      <c r="O34" s="25">
+        <v>2742607</v>
+      </c>
+      <c r="P34" s="25">
+        <v>2795486</v>
+      </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
@@ -2221,15 +2281,15 @@
       </c>
       <c r="N37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>352970</v>
       </c>
       <c r="O37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>346457</v>
       </c>
       <c r="P37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>346628</v>
       </c>
       <c r="Q37" s="32">
         <f t="shared" si="8"/>
@@ -2274,15 +2334,15 @@
       </c>
       <c r="N38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>261996</v>
       </c>
       <c r="O38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>256175</v>
       </c>
       <c r="P38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>256172</v>
       </c>
       <c r="Q38" s="34">
         <f t="shared" si="9"/>
@@ -2319,9 +2379,15 @@
       <c r="M39" s="35">
         <v>254336</v>
       </c>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
+      <c r="N39" s="35">
+        <v>261860</v>
+      </c>
+      <c r="O39" s="35">
+        <v>256039</v>
+      </c>
+      <c r="P39" s="35">
+        <v>256036</v>
+      </c>
       <c r="Q39" s="35"/>
       <c r="R39" s="35"/>
       <c r="S39" s="35"/>
@@ -2348,9 +2414,15 @@
       <c r="M40" s="35">
         <v>136</v>
       </c>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
+      <c r="N40" s="35">
+        <v>136</v>
+      </c>
+      <c r="O40" s="35">
+        <v>136</v>
+      </c>
+      <c r="P40" s="35">
+        <v>136</v>
+      </c>
       <c r="Q40" s="35"/>
       <c r="R40" s="35"/>
       <c r="S40" s="35"/>
@@ -2402,15 +2474,15 @@
       </c>
       <c r="N42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>90974</v>
       </c>
       <c r="O42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>90282</v>
       </c>
       <c r="P42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>90456</v>
       </c>
       <c r="Q42" s="34">
         <f t="shared" si="9"/>
@@ -2447,6 +2519,15 @@
       <c r="M43" s="35">
         <v>85813</v>
       </c>
+      <c r="N43" s="35">
+        <v>85998</v>
+      </c>
+      <c r="O43" s="35">
+        <v>85404</v>
+      </c>
+      <c r="P43" s="35">
+        <v>85483</v>
+      </c>
     </row>
     <row r="44" spans="1:19" s="35" customFormat="1" ht="12.75" customHeight="1">
       <c r="E44" s="35" t="s">
@@ -2469,6 +2550,15 @@
       </c>
       <c r="M44" s="35">
         <v>4822</v>
+      </c>
+      <c r="N44" s="35">
+        <v>4976</v>
+      </c>
+      <c r="O44" s="35">
+        <v>4878</v>
+      </c>
+      <c r="P44" s="35">
+        <v>4973</v>
       </c>
     </row>
     <row r="47" spans="1:19">

</xml_diff>

<commit_message>
Q4 2025 SNA Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
+++ b/Data/Fiscal Data/BTr-Monthly-Debt-Stock-2009-to-current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F5817F-ADCD-41C9-BB61-A965D01458E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3137061-85DE-4180-B2FE-BC2DB3013E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1890" windowWidth="14715" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-510" yWindow="360" windowWidth="14715" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="17" r:id="rId1"/>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3273FFF-38CF-4648-BAF5-82868DEFDB4E}">
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="I6" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42:S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1230,15 +1230,15 @@
       </c>
       <c r="Q8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17906552</v>
       </c>
       <c r="R8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18004021</v>
       </c>
       <c r="S8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18052386</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="14" customFormat="1">
@@ -1302,15 +1302,15 @@
       </c>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17562138</v>
       </c>
       <c r="R10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17647979</v>
       </c>
       <c r="S10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17707814</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="6.95" customHeight="1">
@@ -1379,15 +1379,15 @@
       </c>
       <c r="Q12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12045325</v>
       </c>
       <c r="R12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12117056</v>
       </c>
       <c r="S12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12116253</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1436,15 +1436,15 @@
       </c>
       <c r="Q13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="R13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="S13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1493,15 +1493,15 @@
       </c>
       <c r="Q14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="R14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="S14" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1539,9 +1539,15 @@
       <c r="P15" s="23">
         <v>156</v>
       </c>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
+      <c r="Q15" s="23">
+        <v>156</v>
+      </c>
+      <c r="R15" s="23">
+        <v>156</v>
+      </c>
+      <c r="S15" s="23">
+        <v>156</v>
+      </c>
     </row>
     <row r="16" spans="1:19">
       <c r="C16" s="21"/>
@@ -1578,9 +1584,15 @@
       <c r="P16" s="23">
         <v>156</v>
       </c>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
+      <c r="Q16" s="23">
+        <v>156</v>
+      </c>
+      <c r="R16" s="23">
+        <v>156</v>
+      </c>
+      <c r="S16" s="23">
+        <v>156</v>
+      </c>
     </row>
     <row r="17" spans="3:19">
       <c r="C17" s="21"/>
@@ -1617,9 +1629,15 @@
       <c r="P17" s="23">
         <v>0</v>
       </c>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
+      <c r="Q17" s="23">
+        <v>0</v>
+      </c>
+      <c r="R17" s="23">
+        <v>0</v>
+      </c>
+      <c r="S17" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="3:19">
       <c r="C18" s="21"/>
@@ -1656,9 +1674,15 @@
       <c r="P18" s="23">
         <v>0</v>
       </c>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
+      <c r="Q18" s="23">
+        <v>0</v>
+      </c>
+      <c r="R18" s="23">
+        <v>0</v>
+      </c>
+      <c r="S18" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="3:19">
       <c r="C19" s="21"/>
@@ -1695,9 +1719,15 @@
       <c r="P19" s="22">
         <v>0</v>
       </c>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
+      <c r="Q19" s="22">
+        <v>0</v>
+      </c>
+      <c r="R19" s="22">
+        <v>0</v>
+      </c>
+      <c r="S19" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="3:19">
       <c r="C20" s="21"/>
@@ -1857,9 +1887,15 @@
       <c r="P25" s="25">
         <v>11972744</v>
       </c>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
+      <c r="Q25" s="25">
+        <v>12045169</v>
+      </c>
+      <c r="R25" s="25">
+        <v>12116900</v>
+      </c>
+      <c r="S25" s="25">
+        <v>12116097</v>
+      </c>
     </row>
     <row r="26" spans="3:19">
       <c r="C26" s="21"/>
@@ -1926,15 +1962,15 @@
       </c>
       <c r="Q27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5516813</v>
       </c>
       <c r="R27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5530923</v>
       </c>
       <c r="S27" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5591561</v>
       </c>
     </row>
     <row r="28" spans="3:19" s="24" customFormat="1">
@@ -1983,15 +2019,15 @@
       </c>
       <c r="Q28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2698939</v>
       </c>
       <c r="R28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2714467</v>
       </c>
       <c r="S28" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2769078</v>
       </c>
     </row>
     <row r="29" spans="3:19">
@@ -2040,15 +2076,15 @@
       </c>
       <c r="Q29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2698939</v>
       </c>
       <c r="R29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2714467</v>
       </c>
       <c r="S29" s="26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2769078</v>
       </c>
     </row>
     <row r="30" spans="3:19">
@@ -2086,9 +2122,15 @@
       <c r="P30" s="25">
         <v>2678149</v>
       </c>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
+      <c r="Q30" s="25">
+        <v>2690550</v>
+      </c>
+      <c r="R30" s="25">
+        <v>2706193</v>
+      </c>
+      <c r="S30" s="25">
+        <v>2760856</v>
+      </c>
     </row>
     <row r="31" spans="3:19">
       <c r="C31" s="21"/>
@@ -2125,9 +2167,15 @@
       <c r="P31" s="25">
         <v>8824</v>
       </c>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
+      <c r="Q31" s="25">
+        <v>8389</v>
+      </c>
+      <c r="R31" s="25">
+        <v>8274</v>
+      </c>
+      <c r="S31" s="25">
+        <v>8222</v>
+      </c>
     </row>
     <row r="32" spans="3:19">
       <c r="C32" s="21"/>
@@ -2164,9 +2212,15 @@
       <c r="P32" s="22">
         <v>0</v>
       </c>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
+      <c r="Q32" s="22">
+        <v>0</v>
+      </c>
+      <c r="R32" s="22">
+        <v>0</v>
+      </c>
+      <c r="S32" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:19" ht="6.95" customHeight="1">
       <c r="C33" s="21"/>
@@ -2222,9 +2276,15 @@
       <c r="P34" s="25">
         <v>2795486</v>
       </c>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="25"/>
-      <c r="S34" s="25"/>
+      <c r="Q34" s="25">
+        <v>2817874</v>
+      </c>
+      <c r="R34" s="25">
+        <v>2816456</v>
+      </c>
+      <c r="S34" s="25">
+        <v>2822483</v>
+      </c>
     </row>
     <row r="35" spans="1:19">
       <c r="C35" s="19"/>
@@ -2293,15 +2353,15 @@
       </c>
       <c r="Q37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>344414</v>
       </c>
       <c r="R37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>356042</v>
       </c>
       <c r="S37" s="32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>344572</v>
       </c>
     </row>
     <row r="38" spans="1:19" s="33" customFormat="1" ht="14.25" customHeight="1">
@@ -2346,15 +2406,15 @@
       </c>
       <c r="Q38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>254920</v>
       </c>
       <c r="R38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>267628</v>
       </c>
       <c r="S38" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>256732</v>
       </c>
     </row>
     <row r="39" spans="1:19" s="24" customFormat="1">
@@ -2388,9 +2448,15 @@
       <c r="P39" s="35">
         <v>256036</v>
       </c>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
-      <c r="S39" s="35"/>
+      <c r="Q39" s="35">
+        <v>254784</v>
+      </c>
+      <c r="R39" s="35">
+        <v>267492</v>
+      </c>
+      <c r="S39" s="35">
+        <v>256596</v>
+      </c>
     </row>
     <row r="40" spans="1:19" s="24" customFormat="1" ht="12.75" customHeight="1">
       <c r="E40" s="24" t="s">
@@ -2423,9 +2489,15 @@
       <c r="P40" s="35">
         <v>136</v>
       </c>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
+      <c r="Q40" s="35">
+        <v>136</v>
+      </c>
+      <c r="R40" s="35">
+        <v>136</v>
+      </c>
+      <c r="S40" s="35">
+        <v>136</v>
+      </c>
     </row>
     <row r="41" spans="1:19">
       <c r="E41" s="14"/>
@@ -2486,15 +2558,15 @@
       </c>
       <c r="Q42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>89494</v>
       </c>
       <c r="R42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>88414</v>
       </c>
       <c r="S42" s="34">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>87840</v>
       </c>
     </row>
     <row r="43" spans="1:19" s="35" customFormat="1">
@@ -2528,6 +2600,15 @@
       <c r="P43" s="35">
         <v>85483</v>
       </c>
+      <c r="Q43" s="35">
+        <v>84468</v>
+      </c>
+      <c r="R43" s="35">
+        <v>83392</v>
+      </c>
+      <c r="S43" s="35">
+        <v>82812</v>
+      </c>
     </row>
     <row r="44" spans="1:19" s="35" customFormat="1" ht="12.75" customHeight="1">
       <c r="E44" s="35" t="s">
@@ -2559,6 +2640,15 @@
       </c>
       <c r="P44" s="35">
         <v>4973</v>
+      </c>
+      <c r="Q44" s="35">
+        <v>5026</v>
+      </c>
+      <c r="R44" s="35">
+        <v>5022</v>
+      </c>
+      <c r="S44" s="35">
+        <v>5028</v>
       </c>
     </row>
     <row r="47" spans="1:19">

</xml_diff>